<commit_message>
update for OP accesscnt-daily-bymachine
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/accesscnt-daily-bymachine.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/accesscnt-daily-bymachine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -268,18 +268,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>root</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interhui</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>crm_tomcat_pangu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SELECT hostname, count(*) from ${moduleName} where ts &gt;= DATE_ADD('${selectedDate} 00:00:00',INTERVAL -1 DAY) and ts &lt;= DATE_ADD('${selectedDate} 23:59:59', INTERVAL -1 DAY) group by hostname;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -289,6 +277,21 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crm123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crm_tomcat_pss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1145,11 +1148,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="85657472"/>
-        <c:axId val="85659008"/>
+        <c:axId val="79799424"/>
+        <c:axId val="79800960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85657472"/>
+        <c:axId val="79799424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1158,14 +1161,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85659008"/>
+        <c:crossAx val="79800960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85659008"/>
+        <c:axId val="79800960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,14 +1177,13 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85657472"/>
+        <c:crossAx val="79799424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1192,7 +1194,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.7500000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001188" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001188" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1572,9 +1574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
   <cols>
@@ -1731,7 +1735,7 @@
     </row>
     <row r="28" spans="1:13" ht="16.5" customHeight="1">
       <c r="A28" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B28" s="37" t="str">
         <f>_input!$C12</f>
@@ -1776,6 +1780,11 @@
       <c r="M28" s="43">
         <f>_input!$J12</f>
         <v>47816</v>
+      </c>
+    </row>
+    <row r="37" spans="14:14">
+      <c r="N37" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1817,9 +1826,7 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1845,7 +1852,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1853,7 +1860,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1917,7 +1924,7 @@
         <v>49</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>50</v>
@@ -1961,7 +1968,7 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -2467,7 +2474,7 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2485,7 +2492,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" thickBot="1">
@@ -2504,7 +2511,6 @@
         <v>45583</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2537,7 +2543,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" thickBot="1">

</xml_diff>